<commit_message>
Time seems to be working, making input a bit better
</commit_message>
<xml_diff>
--- a/sheets/input/tests/testy_test.xlsx
+++ b/sheets/input/tests/testy_test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="9740" yWindow="0" windowWidth="23140" windowHeight="20140" tabRatio="741"/>
+    <workbookView xWindow="-520" yWindow="-460" windowWidth="28840" windowHeight="18000" tabRatio="741" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Model_param" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="91">
   <si>
     <t>Number of Hyper-cube bins</t>
   </si>
@@ -252,9 +252,6 @@
     <t>Steady State</t>
   </si>
   <si>
-    <t>YES</t>
-  </si>
-  <si>
     <t>If you are not going to use any probability distrubtions as input set variablity iterations, and Uncertainty iterations both 1</t>
   </si>
   <si>
@@ -262,9 +259,6 @@
   </si>
   <si>
     <t>and Beginning and Ending Date must be the same.</t>
-  </si>
-  <si>
-    <t>Date 2</t>
   </si>
   <si>
     <t>If you would like to solve a steady state problem, you must set Steady State to "YES", and only define one region,</t>
@@ -279,7 +273,31 @@
     <t>Day</t>
   </si>
   <si>
-    <t>11,11,2012</t>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>V, Normal</t>
+  </si>
+  <si>
+    <t>5,12,2012</t>
+  </si>
+  <si>
+    <t>5,20,2012</t>
+  </si>
+  <si>
+    <t>0.005, 0.00005</t>
+  </si>
+  <si>
+    <t>V, Beta</t>
+  </si>
+  <si>
+    <t>2,2</t>
+  </si>
+  <si>
+    <t>5,3</t>
+  </si>
+  <si>
+    <t>V, Weibull</t>
   </si>
 </sst>
 </file>
@@ -292,7 +310,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -561,10 +578,80 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="245">
+  <cellStyleXfs count="315">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -895,7 +982,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="245">
+  <cellStyles count="315">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1018,6 +1105,41 @@
     <cellStyle name="Followed Hyperlink" xfId="240" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="242" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="244" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="246" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="248" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="250" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="252" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="254" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="256" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="258" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="260" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="262" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="264" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="266" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="268" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="270" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="272" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="274" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="276" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="278" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="280" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="282" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="284" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="286" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="288" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="290" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="292" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="294" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="296" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="298" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="300" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="302" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="304" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="306" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="308" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="310" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="312" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="314" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1140,6 +1262,41 @@
     <cellStyle name="Hyperlink" xfId="239" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="241" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="243" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="245" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="247" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="249" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="251" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="253" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="255" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="257" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="259" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="261" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="263" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="265" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="267" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="269" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="271" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="273" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="275" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="277" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="279" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="281" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="283" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="285" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="287" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="289" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="291" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="293" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="295" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="297" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="299" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="301" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="303" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="305" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="307" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="309" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="311" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="313" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1471,8 +1628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1494,25 +1651,25 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="28" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B2" s="29">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="C2" s="55" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D2" s="55"/>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="28" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B3" s="29">
         <v>1</v>
       </c>
       <c r="C3" s="35" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D3" s="35"/>
     </row>
@@ -1524,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="35" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D4" s="35"/>
     </row>
@@ -1533,7 +1690,7 @@
         <v>61</v>
       </c>
       <c r="C5" s="35" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1549,7 +1706,7 @@
         <v>63</v>
       </c>
       <c r="B7" s="52" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1557,7 +1714,7 @@
         <v>64</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1570,7 +1727,7 @@
         <v>74</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -1592,7 +1749,7 @@
   <dimension ref="A1:J77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C6"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2075,10 +2232,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:NE5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="U3" sqref="U3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2086,11 +2243,199 @@
     <col min="1" max="1" width="25" customWidth="1"/>
     <col min="2" max="2" width="21.1640625" customWidth="1"/>
     <col min="3" max="3" width="22.33203125" customWidth="1"/>
-    <col min="4" max="4" width="21.33203125" customWidth="1"/>
-    <col min="5" max="5" width="22.33203125" customWidth="1"/>
+    <col min="4" max="4" width="21.1640625" style="17" customWidth="1"/>
+    <col min="5" max="5" width="22.33203125" style="17" customWidth="1"/>
+    <col min="6" max="6" width="21.1640625" style="17" customWidth="1"/>
+    <col min="7" max="7" width="22.33203125" style="17" customWidth="1"/>
+    <col min="8" max="8" width="21.1640625" style="17" customWidth="1"/>
+    <col min="9" max="9" width="22.33203125" style="17" customWidth="1"/>
+    <col min="10" max="10" width="21.1640625" style="17" customWidth="1"/>
+    <col min="11" max="11" width="22.33203125" style="17" customWidth="1"/>
+    <col min="12" max="12" width="21.1640625" style="17" customWidth="1"/>
+    <col min="13" max="13" width="22.33203125" style="17" customWidth="1"/>
+    <col min="14" max="14" width="21.1640625" style="17" customWidth="1"/>
+    <col min="15" max="15" width="22.33203125" style="17" customWidth="1"/>
+    <col min="16" max="16" width="21.1640625" style="17" customWidth="1"/>
+    <col min="17" max="17" width="22.33203125" style="17" customWidth="1"/>
+    <col min="18" max="18" width="21.1640625" style="17" customWidth="1"/>
+    <col min="19" max="19" width="22.33203125" style="17" customWidth="1"/>
+    <col min="20" max="20" width="21.33203125" style="17" customWidth="1"/>
+    <col min="21" max="21" width="22.33203125" style="17" customWidth="1"/>
+    <col min="22" max="22" width="21.1640625" style="17" customWidth="1"/>
+    <col min="23" max="23" width="22.33203125" style="17" customWidth="1"/>
+    <col min="24" max="24" width="21.33203125" style="17" customWidth="1"/>
+    <col min="25" max="25" width="22.33203125" style="17" customWidth="1"/>
+    <col min="26" max="26" width="21.1640625" style="17" customWidth="1"/>
+    <col min="27" max="27" width="22.33203125" style="17" customWidth="1"/>
+    <col min="28" max="28" width="21.33203125" style="17" customWidth="1"/>
+    <col min="29" max="29" width="22.33203125" style="17" customWidth="1"/>
+    <col min="30" max="30" width="21.1640625" style="17" customWidth="1"/>
+    <col min="31" max="31" width="22.33203125" style="17" customWidth="1"/>
+    <col min="32" max="32" width="21.33203125" style="17" customWidth="1"/>
+    <col min="33" max="33" width="22.33203125" style="17" customWidth="1"/>
+    <col min="34" max="34" width="21.1640625" style="17" customWidth="1"/>
+    <col min="35" max="35" width="22.33203125" style="17" customWidth="1"/>
+    <col min="36" max="36" width="21.33203125" style="17" customWidth="1"/>
+    <col min="37" max="37" width="22.33203125" style="17" customWidth="1"/>
+    <col min="38" max="38" width="21.1640625" style="17" customWidth="1"/>
+    <col min="39" max="39" width="22.33203125" style="17" customWidth="1"/>
+    <col min="40" max="40" width="21.33203125" style="17" customWidth="1"/>
+    <col min="41" max="41" width="22.33203125" style="17" customWidth="1"/>
+    <col min="42" max="42" width="21.1640625" style="17" customWidth="1"/>
+    <col min="43" max="43" width="22.33203125" style="17" customWidth="1"/>
+    <col min="44" max="44" width="21.33203125" style="17" customWidth="1"/>
+    <col min="45" max="45" width="22.33203125" style="17" customWidth="1"/>
+    <col min="46" max="46" width="21.1640625" style="17" customWidth="1"/>
+    <col min="47" max="47" width="22.33203125" style="17" customWidth="1"/>
+    <col min="48" max="48" width="21.33203125" style="17" customWidth="1"/>
+    <col min="49" max="49" width="22.33203125" style="17" customWidth="1"/>
+    <col min="50" max="50" width="21.1640625" style="17" customWidth="1"/>
+    <col min="51" max="51" width="22.33203125" style="17" customWidth="1"/>
+    <col min="52" max="52" width="21.33203125" style="17" customWidth="1"/>
+    <col min="53" max="53" width="22.33203125" style="17" customWidth="1"/>
+    <col min="54" max="54" width="21.1640625" style="17" customWidth="1"/>
+    <col min="55" max="55" width="22.33203125" style="17" customWidth="1"/>
+    <col min="56" max="56" width="21.33203125" style="17" customWidth="1"/>
+    <col min="57" max="57" width="22.33203125" style="17" customWidth="1"/>
+    <col min="58" max="58" width="21.1640625" style="17" customWidth="1"/>
+    <col min="59" max="59" width="22.33203125" style="17" customWidth="1"/>
+    <col min="60" max="60" width="21.33203125" style="17" customWidth="1"/>
+    <col min="61" max="61" width="22.33203125" style="17" customWidth="1"/>
+    <col min="62" max="62" width="21.1640625" style="17" customWidth="1"/>
+    <col min="63" max="63" width="22.33203125" style="17" customWidth="1"/>
+    <col min="64" max="64" width="21.33203125" style="17" customWidth="1"/>
+    <col min="65" max="65" width="22.33203125" style="17" customWidth="1"/>
+    <col min="66" max="66" width="21.1640625" style="17" customWidth="1"/>
+    <col min="67" max="67" width="22.33203125" style="17" customWidth="1"/>
+    <col min="68" max="68" width="21.33203125" style="17" customWidth="1"/>
+    <col min="69" max="69" width="22.33203125" style="17" customWidth="1"/>
+    <col min="70" max="70" width="21.1640625" style="17" customWidth="1"/>
+    <col min="71" max="71" width="22.33203125" style="17" customWidth="1"/>
+    <col min="72" max="72" width="21.33203125" style="17" customWidth="1"/>
+    <col min="73" max="73" width="22.33203125" style="17" customWidth="1"/>
+    <col min="74" max="74" width="21.1640625" style="17" customWidth="1"/>
+    <col min="75" max="75" width="22.33203125" style="17" customWidth="1"/>
+    <col min="76" max="76" width="21.33203125" style="17" customWidth="1"/>
+    <col min="77" max="77" width="22.33203125" style="17" customWidth="1"/>
+    <col min="78" max="78" width="21.1640625" style="17" customWidth="1"/>
+    <col min="79" max="79" width="22.33203125" style="17" customWidth="1"/>
+    <col min="80" max="80" width="21.33203125" style="17" customWidth="1"/>
+    <col min="81" max="81" width="22.33203125" style="17" customWidth="1"/>
+    <col min="82" max="82" width="21.1640625" style="17" customWidth="1"/>
+    <col min="83" max="83" width="22.33203125" style="17" customWidth="1"/>
+    <col min="84" max="84" width="21.33203125" style="17" customWidth="1"/>
+    <col min="85" max="85" width="22.33203125" style="17" customWidth="1"/>
+    <col min="86" max="86" width="21.1640625" style="17" customWidth="1"/>
+    <col min="87" max="87" width="22.33203125" style="17" customWidth="1"/>
+    <col min="88" max="88" width="21.33203125" style="17" customWidth="1"/>
+    <col min="89" max="89" width="22.33203125" style="17" customWidth="1"/>
+    <col min="90" max="90" width="21.1640625" style="17" customWidth="1"/>
+    <col min="91" max="91" width="22.33203125" style="17" customWidth="1"/>
+    <col min="92" max="92" width="21.33203125" style="17" customWidth="1"/>
+    <col min="93" max="93" width="22.33203125" style="17" customWidth="1"/>
+    <col min="94" max="94" width="21.1640625" style="17" customWidth="1"/>
+    <col min="95" max="95" width="22.33203125" style="17" customWidth="1"/>
+    <col min="96" max="96" width="21.33203125" style="17" customWidth="1"/>
+    <col min="97" max="97" width="22.33203125" style="17" customWidth="1"/>
+    <col min="98" max="98" width="21.1640625" style="17" customWidth="1"/>
+    <col min="99" max="99" width="22.33203125" style="17" customWidth="1"/>
+    <col min="100" max="100" width="21.33203125" style="17" customWidth="1"/>
+    <col min="101" max="101" width="22.33203125" style="17" customWidth="1"/>
+    <col min="102" max="102" width="21.1640625" style="17" customWidth="1"/>
+    <col min="103" max="103" width="22.33203125" style="17" customWidth="1"/>
+    <col min="104" max="104" width="21.33203125" style="17" customWidth="1"/>
+    <col min="105" max="105" width="22.33203125" style="17" customWidth="1"/>
+    <col min="106" max="106" width="21.1640625" style="17" customWidth="1"/>
+    <col min="107" max="107" width="22.33203125" style="17" customWidth="1"/>
+    <col min="108" max="108" width="21.33203125" style="17" customWidth="1"/>
+    <col min="109" max="109" width="22.33203125" style="17" customWidth="1"/>
+    <col min="110" max="110" width="21.1640625" style="17" customWidth="1"/>
+    <col min="111" max="111" width="22.33203125" style="17" customWidth="1"/>
+    <col min="112" max="112" width="21.33203125" style="17" customWidth="1"/>
+    <col min="113" max="113" width="22.33203125" style="17" customWidth="1"/>
+    <col min="114" max="114" width="21.1640625" style="17" customWidth="1"/>
+    <col min="115" max="115" width="22.33203125" style="17" customWidth="1"/>
+    <col min="116" max="116" width="21.33203125" style="17" customWidth="1"/>
+    <col min="117" max="117" width="22.33203125" style="17" customWidth="1"/>
+    <col min="118" max="118" width="21.1640625" style="17" customWidth="1"/>
+    <col min="119" max="119" width="22.33203125" style="17" customWidth="1"/>
+    <col min="120" max="120" width="21.33203125" style="17" customWidth="1"/>
+    <col min="121" max="121" width="22.33203125" style="17" customWidth="1"/>
+    <col min="122" max="122" width="21.1640625" style="17" customWidth="1"/>
+    <col min="123" max="123" width="22.33203125" style="17" customWidth="1"/>
+    <col min="124" max="124" width="21.33203125" style="17" customWidth="1"/>
+    <col min="125" max="125" width="22.33203125" style="17" customWidth="1"/>
+    <col min="126" max="126" width="21.1640625" style="17" customWidth="1"/>
+    <col min="127" max="127" width="22.33203125" style="17" customWidth="1"/>
+    <col min="128" max="128" width="21.33203125" style="17" customWidth="1"/>
+    <col min="129" max="129" width="22.33203125" style="17" customWidth="1"/>
+    <col min="130" max="130" width="21.1640625" style="17" customWidth="1"/>
+    <col min="131" max="131" width="22.33203125" style="17" customWidth="1"/>
+    <col min="132" max="132" width="21.33203125" style="17" customWidth="1"/>
+    <col min="133" max="133" width="22.33203125" style="17" customWidth="1"/>
+    <col min="134" max="134" width="21.1640625" style="17" customWidth="1"/>
+    <col min="135" max="135" width="22.33203125" style="17" customWidth="1"/>
+    <col min="136" max="136" width="21.33203125" style="17" customWidth="1"/>
+    <col min="137" max="137" width="22.33203125" style="17" customWidth="1"/>
+    <col min="138" max="138" width="21.1640625" style="17" customWidth="1"/>
+    <col min="139" max="139" width="22.33203125" style="17" customWidth="1"/>
+    <col min="140" max="140" width="21.33203125" style="17" customWidth="1"/>
+    <col min="141" max="141" width="22.33203125" style="17" customWidth="1"/>
+    <col min="142" max="142" width="21.1640625" style="17" customWidth="1"/>
+    <col min="143" max="143" width="22.33203125" style="17" customWidth="1"/>
+    <col min="144" max="144" width="21.33203125" style="17" customWidth="1"/>
+    <col min="145" max="145" width="22.33203125" style="17" customWidth="1"/>
+    <col min="146" max="146" width="21.1640625" style="17" customWidth="1"/>
+    <col min="147" max="147" width="22.33203125" style="17" customWidth="1"/>
+    <col min="148" max="148" width="21.33203125" style="17" customWidth="1"/>
+    <col min="149" max="149" width="22.33203125" style="17" customWidth="1"/>
+    <col min="150" max="150" width="21.1640625" style="17" customWidth="1"/>
+    <col min="151" max="151" width="22.33203125" style="17" customWidth="1"/>
+    <col min="152" max="152" width="21.33203125" style="17" customWidth="1"/>
+    <col min="153" max="153" width="22.33203125" style="17" customWidth="1"/>
+    <col min="154" max="154" width="21.1640625" style="17" customWidth="1"/>
+    <col min="155" max="155" width="22.33203125" style="17" customWidth="1"/>
+    <col min="156" max="156" width="21.33203125" style="17" customWidth="1"/>
+    <col min="157" max="157" width="22.33203125" style="17" customWidth="1"/>
+    <col min="158" max="158" width="21.1640625" style="17" customWidth="1"/>
+    <col min="159" max="159" width="22.33203125" style="17" customWidth="1"/>
+    <col min="160" max="160" width="21.33203125" style="17" customWidth="1"/>
+    <col min="161" max="161" width="22.33203125" style="17" customWidth="1"/>
+    <col min="162" max="162" width="21.1640625" style="17" customWidth="1"/>
+    <col min="163" max="163" width="22.33203125" style="17" customWidth="1"/>
+    <col min="164" max="164" width="21.33203125" style="17" customWidth="1"/>
+    <col min="165" max="165" width="22.33203125" style="17" customWidth="1"/>
+    <col min="166" max="166" width="21.1640625" style="17" customWidth="1"/>
+    <col min="167" max="167" width="22.33203125" style="17" customWidth="1"/>
+    <col min="168" max="168" width="21.33203125" style="17" customWidth="1"/>
+    <col min="169" max="169" width="22.33203125" style="17" customWidth="1"/>
+    <col min="170" max="170" width="21.1640625" style="17" customWidth="1"/>
+    <col min="171" max="171" width="22.33203125" style="17" customWidth="1"/>
+    <col min="172" max="172" width="21.33203125" style="17" customWidth="1"/>
+    <col min="173" max="173" width="22.33203125" style="17" customWidth="1"/>
+    <col min="174" max="174" width="21.1640625" style="17" customWidth="1"/>
+    <col min="175" max="175" width="22.33203125" style="17" customWidth="1"/>
+    <col min="176" max="176" width="21.33203125" style="17" customWidth="1"/>
+    <col min="177" max="177" width="22.33203125" style="17" customWidth="1"/>
+    <col min="178" max="178" width="21.1640625" style="17" customWidth="1"/>
+    <col min="179" max="179" width="22.33203125" style="17" customWidth="1"/>
+    <col min="180" max="180" width="21.33203125" style="17" customWidth="1"/>
+    <col min="181" max="181" width="22.33203125" style="17" customWidth="1"/>
+    <col min="182" max="182" width="21.1640625" style="17" customWidth="1"/>
+    <col min="183" max="183" width="22.33203125" style="17" customWidth="1"/>
+    <col min="184" max="184" width="21.33203125" style="17" customWidth="1"/>
+    <col min="185" max="185" width="22.33203125" style="17" customWidth="1"/>
+    <col min="186" max="186" width="21.1640625" style="17" customWidth="1"/>
+    <col min="187" max="187" width="22.33203125" style="17" customWidth="1"/>
+    <col min="188" max="188" width="21.33203125" style="17" customWidth="1"/>
+    <col min="189" max="189" width="22.33203125" style="17" customWidth="1"/>
+    <col min="190" max="190" width="21.1640625" style="17" customWidth="1"/>
+    <col min="191" max="191" width="22.33203125" style="17" customWidth="1"/>
+    <col min="192" max="192" width="21.33203125" style="17" customWidth="1"/>
+    <col min="193" max="193" width="22.33203125" style="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:369">
       <c r="A1" s="58" t="s">
         <v>65</v>
       </c>
@@ -2099,11 +2444,387 @@
       </c>
       <c r="C1" s="62"/>
       <c r="D1" s="60" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="E1" s="62"/>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="60" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1" s="62"/>
+      <c r="H1" s="60" t="s">
+        <v>67</v>
+      </c>
+      <c r="I1" s="62"/>
+      <c r="J1" s="60" t="s">
+        <v>67</v>
+      </c>
+      <c r="K1" s="62"/>
+      <c r="L1" s="60" t="s">
+        <v>67</v>
+      </c>
+      <c r="M1" s="62"/>
+      <c r="N1" s="60" t="s">
+        <v>67</v>
+      </c>
+      <c r="O1" s="62"/>
+      <c r="P1" s="60" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q1" s="62"/>
+      <c r="R1" s="60"/>
+      <c r="S1" s="62"/>
+      <c r="T1" s="60"/>
+      <c r="U1" s="62"/>
+      <c r="V1" s="60"/>
+      <c r="W1" s="62"/>
+      <c r="X1" s="60"/>
+      <c r="Y1" s="62"/>
+      <c r="Z1" s="60"/>
+      <c r="AA1" s="62"/>
+      <c r="AB1" s="60"/>
+      <c r="AC1" s="62"/>
+      <c r="AD1" s="60"/>
+      <c r="AE1" s="62"/>
+      <c r="AF1" s="60"/>
+      <c r="AG1" s="62"/>
+      <c r="AH1" s="60"/>
+      <c r="AI1" s="62"/>
+      <c r="AJ1" s="60"/>
+      <c r="AK1" s="62"/>
+      <c r="AL1" s="60"/>
+      <c r="AM1" s="62"/>
+      <c r="AN1" s="60"/>
+      <c r="AO1" s="62"/>
+      <c r="AP1" s="60"/>
+      <c r="AQ1" s="62"/>
+      <c r="AR1" s="60"/>
+      <c r="AS1" s="62"/>
+      <c r="AT1" s="60"/>
+      <c r="AU1" s="62"/>
+      <c r="AV1" s="60"/>
+      <c r="AW1" s="62"/>
+      <c r="AX1" s="60"/>
+      <c r="AY1" s="62"/>
+      <c r="AZ1" s="60"/>
+      <c r="BA1" s="62"/>
+      <c r="BB1" s="60"/>
+      <c r="BC1" s="62"/>
+      <c r="BD1" s="60"/>
+      <c r="BE1" s="62"/>
+      <c r="BF1" s="60"/>
+      <c r="BG1" s="62"/>
+      <c r="BH1" s="60"/>
+      <c r="BI1" s="62"/>
+      <c r="BJ1" s="60"/>
+      <c r="BK1" s="62"/>
+      <c r="BL1" s="60"/>
+      <c r="BM1" s="62"/>
+      <c r="BN1" s="60"/>
+      <c r="BO1" s="62"/>
+      <c r="BP1" s="60"/>
+      <c r="BQ1" s="62"/>
+      <c r="BR1" s="60"/>
+      <c r="BS1" s="62"/>
+      <c r="BT1" s="60"/>
+      <c r="BU1" s="62"/>
+      <c r="BV1" s="60"/>
+      <c r="BW1" s="62"/>
+      <c r="BX1" s="60"/>
+      <c r="BY1" s="62"/>
+      <c r="BZ1" s="60"/>
+      <c r="CA1" s="62"/>
+      <c r="CB1" s="60"/>
+      <c r="CC1" s="62"/>
+      <c r="CD1" s="60"/>
+      <c r="CE1" s="62"/>
+      <c r="CF1" s="60"/>
+      <c r="CG1" s="62"/>
+      <c r="CH1" s="60"/>
+      <c r="CI1" s="62"/>
+      <c r="CJ1" s="60"/>
+      <c r="CK1" s="62"/>
+      <c r="CL1" s="60"/>
+      <c r="CM1" s="62"/>
+      <c r="CN1" s="60"/>
+      <c r="CO1" s="62"/>
+      <c r="CP1" s="60"/>
+      <c r="CQ1" s="62"/>
+      <c r="CR1" s="60"/>
+      <c r="CS1" s="62"/>
+      <c r="CT1" s="60"/>
+      <c r="CU1" s="62"/>
+      <c r="CV1" s="60"/>
+      <c r="CW1" s="62"/>
+      <c r="CX1" s="60"/>
+      <c r="CY1" s="62"/>
+      <c r="CZ1" s="60"/>
+      <c r="DA1" s="62"/>
+      <c r="DB1" s="60"/>
+      <c r="DC1" s="62"/>
+      <c r="DD1" s="60"/>
+      <c r="DE1" s="62"/>
+      <c r="DF1" s="60"/>
+      <c r="DG1" s="62"/>
+      <c r="DH1" s="60"/>
+      <c r="DI1" s="62"/>
+      <c r="DJ1" s="60"/>
+      <c r="DK1" s="62"/>
+      <c r="DL1" s="60"/>
+      <c r="DM1" s="62"/>
+      <c r="DN1" s="60"/>
+      <c r="DO1" s="62"/>
+      <c r="DP1" s="60"/>
+      <c r="DQ1" s="62"/>
+      <c r="DR1" s="60"/>
+      <c r="DS1" s="62"/>
+      <c r="DT1" s="60"/>
+      <c r="DU1" s="62"/>
+      <c r="DV1" s="60"/>
+      <c r="DW1" s="62"/>
+      <c r="DX1" s="60"/>
+      <c r="DY1" s="62"/>
+      <c r="DZ1" s="60"/>
+      <c r="EA1" s="62"/>
+      <c r="EB1" s="60"/>
+      <c r="EC1" s="62"/>
+      <c r="ED1" s="60"/>
+      <c r="EE1" s="62"/>
+      <c r="EF1" s="60"/>
+      <c r="EG1" s="62"/>
+      <c r="EH1" s="60"/>
+      <c r="EI1" s="62"/>
+      <c r="EJ1" s="60"/>
+      <c r="EK1" s="62"/>
+      <c r="EL1" s="60"/>
+      <c r="EM1" s="62"/>
+      <c r="EN1" s="60"/>
+      <c r="EO1" s="62"/>
+      <c r="EP1" s="60"/>
+      <c r="EQ1" s="62"/>
+      <c r="ER1" s="60"/>
+      <c r="ES1" s="62"/>
+      <c r="ET1" s="60"/>
+      <c r="EU1" s="62"/>
+      <c r="EV1" s="60"/>
+      <c r="EW1" s="62"/>
+      <c r="EX1" s="60"/>
+      <c r="EY1" s="62"/>
+      <c r="EZ1" s="60"/>
+      <c r="FA1" s="62"/>
+      <c r="FB1" s="60"/>
+      <c r="FC1" s="62"/>
+      <c r="FD1" s="60"/>
+      <c r="FE1" s="62"/>
+      <c r="FF1" s="60"/>
+      <c r="FG1" s="62"/>
+      <c r="FH1" s="60"/>
+      <c r="FI1" s="62"/>
+      <c r="FJ1" s="60"/>
+      <c r="FK1" s="62"/>
+      <c r="FL1" s="60"/>
+      <c r="FM1" s="62"/>
+      <c r="FN1" s="60"/>
+      <c r="FO1" s="62"/>
+      <c r="FP1" s="60"/>
+      <c r="FQ1" s="62"/>
+      <c r="FR1" s="60"/>
+      <c r="FS1" s="62"/>
+      <c r="FT1" s="60"/>
+      <c r="FU1" s="62"/>
+      <c r="FV1" s="60"/>
+      <c r="FW1" s="62"/>
+      <c r="FX1" s="60"/>
+      <c r="FY1" s="62"/>
+      <c r="FZ1" s="60"/>
+      <c r="GA1" s="62"/>
+      <c r="GB1" s="60"/>
+      <c r="GC1" s="62"/>
+      <c r="GD1" s="60"/>
+      <c r="GE1" s="62"/>
+      <c r="GF1" s="60"/>
+      <c r="GG1" s="62"/>
+      <c r="GH1" s="60"/>
+      <c r="GI1" s="62"/>
+      <c r="GJ1" s="60"/>
+      <c r="GK1" s="62"/>
+      <c r="GL1" s="60"/>
+      <c r="GM1" s="62"/>
+      <c r="GN1" s="60"/>
+      <c r="GO1" s="62"/>
+      <c r="GP1" s="60"/>
+      <c r="GQ1" s="62"/>
+      <c r="GR1" s="60"/>
+      <c r="GS1" s="62"/>
+      <c r="GT1" s="60"/>
+      <c r="GU1" s="62"/>
+      <c r="GV1" s="60"/>
+      <c r="GW1" s="62"/>
+      <c r="GX1" s="60"/>
+      <c r="GY1" s="62"/>
+      <c r="GZ1" s="60"/>
+      <c r="HA1" s="62"/>
+      <c r="HB1" s="60"/>
+      <c r="HC1" s="62"/>
+      <c r="HD1" s="60"/>
+      <c r="HE1" s="62"/>
+      <c r="HF1" s="60"/>
+      <c r="HG1" s="62"/>
+      <c r="HH1" s="60"/>
+      <c r="HI1" s="62"/>
+      <c r="HJ1" s="60"/>
+      <c r="HK1" s="62"/>
+      <c r="HL1" s="60"/>
+      <c r="HM1" s="62"/>
+      <c r="HN1" s="60"/>
+      <c r="HO1" s="62"/>
+      <c r="HP1" s="60"/>
+      <c r="HQ1" s="62"/>
+      <c r="HR1" s="60"/>
+      <c r="HS1" s="62"/>
+      <c r="HT1" s="60"/>
+      <c r="HU1" s="62"/>
+      <c r="HV1" s="60"/>
+      <c r="HW1" s="62"/>
+      <c r="HX1" s="60"/>
+      <c r="HY1" s="62"/>
+      <c r="HZ1" s="60"/>
+      <c r="IA1" s="62"/>
+      <c r="IB1" s="60"/>
+      <c r="IC1" s="62"/>
+      <c r="ID1" s="60"/>
+      <c r="IE1" s="62"/>
+      <c r="IF1" s="60"/>
+      <c r="IG1" s="62"/>
+      <c r="IH1" s="60"/>
+      <c r="II1" s="62"/>
+      <c r="IJ1" s="60"/>
+      <c r="IK1" s="62"/>
+      <c r="IL1" s="60"/>
+      <c r="IM1" s="62"/>
+      <c r="IN1" s="60"/>
+      <c r="IO1" s="62"/>
+      <c r="IP1" s="60"/>
+      <c r="IQ1" s="62"/>
+      <c r="IR1" s="60"/>
+      <c r="IS1" s="62"/>
+      <c r="IT1" s="60"/>
+      <c r="IU1" s="62"/>
+      <c r="IV1" s="60"/>
+      <c r="IW1" s="62"/>
+      <c r="IX1" s="60"/>
+      <c r="IY1" s="62"/>
+      <c r="IZ1" s="60"/>
+      <c r="JA1" s="62"/>
+      <c r="JB1" s="60"/>
+      <c r="JC1" s="62"/>
+      <c r="JD1" s="60"/>
+      <c r="JE1" s="62"/>
+      <c r="JF1" s="60"/>
+      <c r="JG1" s="62"/>
+      <c r="JH1" s="60"/>
+      <c r="JI1" s="62"/>
+      <c r="JJ1" s="60"/>
+      <c r="JK1" s="62"/>
+      <c r="JL1" s="60"/>
+      <c r="JM1" s="62"/>
+      <c r="JN1" s="60"/>
+      <c r="JO1" s="62"/>
+      <c r="JP1" s="60"/>
+      <c r="JQ1" s="62"/>
+      <c r="JR1" s="60"/>
+      <c r="JS1" s="62"/>
+      <c r="JT1" s="60"/>
+      <c r="JU1" s="62"/>
+      <c r="JV1" s="60"/>
+      <c r="JW1" s="62"/>
+      <c r="JX1" s="60"/>
+      <c r="JY1" s="62"/>
+      <c r="JZ1" s="60"/>
+      <c r="KA1" s="62"/>
+      <c r="KB1" s="60"/>
+      <c r="KC1" s="62"/>
+      <c r="KD1" s="60"/>
+      <c r="KE1" s="62"/>
+      <c r="KF1" s="60"/>
+      <c r="KG1" s="62"/>
+      <c r="KH1" s="60"/>
+      <c r="KI1" s="62"/>
+      <c r="KJ1" s="60"/>
+      <c r="KK1" s="62"/>
+      <c r="KL1" s="60"/>
+      <c r="KM1" s="62"/>
+      <c r="KN1" s="60"/>
+      <c r="KO1" s="62"/>
+      <c r="KP1" s="60"/>
+      <c r="KQ1" s="62"/>
+      <c r="KR1" s="60"/>
+      <c r="KS1" s="62"/>
+      <c r="KT1" s="60"/>
+      <c r="KU1" s="62"/>
+      <c r="KV1" s="60"/>
+      <c r="KW1" s="62"/>
+      <c r="KX1" s="60"/>
+      <c r="KY1" s="62"/>
+      <c r="KZ1" s="60"/>
+      <c r="LA1" s="62"/>
+      <c r="LB1" s="60"/>
+      <c r="LC1" s="62"/>
+      <c r="LD1" s="60"/>
+      <c r="LE1" s="62"/>
+      <c r="LF1" s="60"/>
+      <c r="LG1" s="62"/>
+      <c r="LH1" s="60"/>
+      <c r="LI1" s="62"/>
+      <c r="LJ1" s="60"/>
+      <c r="LK1" s="62"/>
+      <c r="LL1" s="60"/>
+      <c r="LM1" s="62"/>
+      <c r="LN1" s="60"/>
+      <c r="LO1" s="62"/>
+      <c r="LP1" s="60"/>
+      <c r="LQ1" s="62"/>
+      <c r="LR1" s="60"/>
+      <c r="LS1" s="62"/>
+      <c r="LT1" s="60"/>
+      <c r="LU1" s="62"/>
+      <c r="LV1" s="60"/>
+      <c r="LW1" s="62"/>
+      <c r="LX1" s="60"/>
+      <c r="LY1" s="62"/>
+      <c r="LZ1" s="60"/>
+      <c r="MA1" s="62"/>
+      <c r="MB1" s="60"/>
+      <c r="MC1" s="62"/>
+      <c r="MD1" s="60"/>
+      <c r="ME1" s="62"/>
+      <c r="MF1" s="60"/>
+      <c r="MG1" s="62"/>
+      <c r="MH1" s="60"/>
+      <c r="MI1" s="62"/>
+      <c r="MJ1" s="60"/>
+      <c r="MK1" s="62"/>
+      <c r="ML1" s="60"/>
+      <c r="MM1" s="62"/>
+      <c r="MN1" s="60"/>
+      <c r="MO1" s="62"/>
+      <c r="MP1" s="60"/>
+      <c r="MQ1" s="62"/>
+      <c r="MR1" s="60"/>
+      <c r="MS1" s="62"/>
+      <c r="MT1" s="60"/>
+      <c r="MU1" s="62"/>
+      <c r="MV1" s="60"/>
+      <c r="MW1" s="62"/>
+      <c r="MX1" s="60"/>
+      <c r="MY1" s="62"/>
+      <c r="MZ1" s="60"/>
+      <c r="NA1" s="62"/>
+      <c r="NB1" s="60"/>
+      <c r="NC1" s="62"/>
+      <c r="ND1" s="60"/>
+      <c r="NE1" s="62"/>
+    </row>
+    <row r="2" spans="1:369">
       <c r="A2" s="59"/>
       <c r="B2" s="10" t="s">
         <v>68</v>
@@ -2117,8 +2838,396 @@
       <c r="E2" s="63" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="G2" s="63" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="I2" s="63" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="K2" s="63" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="M2" s="63" t="s">
+        <v>3</v>
+      </c>
+      <c r="N2" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="O2" s="63" t="s">
+        <v>3</v>
+      </c>
+      <c r="P2" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q2" s="63" t="s">
+        <v>3</v>
+      </c>
+      <c r="R2" s="10"/>
+      <c r="S2" s="63"/>
+      <c r="T2" s="10"/>
+      <c r="U2" s="63"/>
+      <c r="V2" s="10"/>
+      <c r="W2" s="63"/>
+      <c r="X2" s="10"/>
+      <c r="Y2" s="63"/>
+      <c r="Z2" s="10"/>
+      <c r="AA2" s="63"/>
+      <c r="AB2" s="10"/>
+      <c r="AC2" s="63"/>
+      <c r="AD2" s="10"/>
+      <c r="AE2" s="63"/>
+      <c r="AF2" s="10"/>
+      <c r="AG2" s="63"/>
+      <c r="AH2" s="10"/>
+      <c r="AI2" s="63"/>
+      <c r="AJ2" s="10"/>
+      <c r="AK2" s="63"/>
+      <c r="AL2" s="10"/>
+      <c r="AM2" s="63"/>
+      <c r="AN2" s="10"/>
+      <c r="AO2" s="63"/>
+      <c r="AP2" s="10"/>
+      <c r="AQ2" s="63"/>
+      <c r="AR2" s="10"/>
+      <c r="AS2" s="63"/>
+      <c r="AT2" s="10"/>
+      <c r="AU2" s="63"/>
+      <c r="AV2" s="10"/>
+      <c r="AW2" s="63"/>
+      <c r="AX2" s="10"/>
+      <c r="AY2" s="63"/>
+      <c r="AZ2" s="10"/>
+      <c r="BA2" s="63"/>
+      <c r="BB2" s="10"/>
+      <c r="BC2" s="63"/>
+      <c r="BD2" s="10"/>
+      <c r="BE2" s="63"/>
+      <c r="BF2" s="10"/>
+      <c r="BG2" s="63"/>
+      <c r="BH2" s="10"/>
+      <c r="BI2" s="63"/>
+      <c r="BJ2" s="10"/>
+      <c r="BK2" s="63"/>
+      <c r="BL2" s="10"/>
+      <c r="BM2" s="63"/>
+      <c r="BN2" s="10"/>
+      <c r="BO2" s="63"/>
+      <c r="BP2" s="10"/>
+      <c r="BQ2" s="63"/>
+      <c r="BR2" s="10"/>
+      <c r="BS2" s="63"/>
+      <c r="BT2" s="10"/>
+      <c r="BU2" s="63"/>
+      <c r="BV2" s="10"/>
+      <c r="BW2" s="63"/>
+      <c r="BX2" s="10"/>
+      <c r="BY2" s="63"/>
+      <c r="BZ2" s="10"/>
+      <c r="CA2" s="63"/>
+      <c r="CB2" s="10"/>
+      <c r="CC2" s="63"/>
+      <c r="CD2" s="10"/>
+      <c r="CE2" s="63"/>
+      <c r="CF2" s="10"/>
+      <c r="CG2" s="63"/>
+      <c r="CH2" s="10"/>
+      <c r="CI2" s="63"/>
+      <c r="CJ2" s="10"/>
+      <c r="CK2" s="63"/>
+      <c r="CL2" s="10"/>
+      <c r="CM2" s="63"/>
+      <c r="CN2" s="10"/>
+      <c r="CO2" s="63"/>
+      <c r="CP2" s="10"/>
+      <c r="CQ2" s="63"/>
+      <c r="CR2" s="10"/>
+      <c r="CS2" s="63"/>
+      <c r="CT2" s="10"/>
+      <c r="CU2" s="63"/>
+      <c r="CV2" s="10"/>
+      <c r="CW2" s="63"/>
+      <c r="CX2" s="10"/>
+      <c r="CY2" s="63"/>
+      <c r="CZ2" s="10"/>
+      <c r="DA2" s="63"/>
+      <c r="DB2" s="10"/>
+      <c r="DC2" s="63"/>
+      <c r="DD2" s="10"/>
+      <c r="DE2" s="63"/>
+      <c r="DF2" s="10"/>
+      <c r="DG2" s="63"/>
+      <c r="DH2" s="10"/>
+      <c r="DI2" s="63"/>
+      <c r="DJ2" s="10"/>
+      <c r="DK2" s="63"/>
+      <c r="DL2" s="10"/>
+      <c r="DM2" s="63"/>
+      <c r="DN2" s="10"/>
+      <c r="DO2" s="63"/>
+      <c r="DP2" s="10"/>
+      <c r="DQ2" s="63"/>
+      <c r="DR2" s="10"/>
+      <c r="DS2" s="63"/>
+      <c r="DT2" s="10"/>
+      <c r="DU2" s="63"/>
+      <c r="DV2" s="10"/>
+      <c r="DW2" s="63"/>
+      <c r="DX2" s="10"/>
+      <c r="DY2" s="63"/>
+      <c r="DZ2" s="10"/>
+      <c r="EA2" s="63"/>
+      <c r="EB2" s="10"/>
+      <c r="EC2" s="63"/>
+      <c r="ED2" s="10"/>
+      <c r="EE2" s="63"/>
+      <c r="EF2" s="10"/>
+      <c r="EG2" s="63"/>
+      <c r="EH2" s="10"/>
+      <c r="EI2" s="63"/>
+      <c r="EJ2" s="10"/>
+      <c r="EK2" s="63"/>
+      <c r="EL2" s="10"/>
+      <c r="EM2" s="63"/>
+      <c r="EN2" s="10"/>
+      <c r="EO2" s="63"/>
+      <c r="EP2" s="10"/>
+      <c r="EQ2" s="63"/>
+      <c r="ER2" s="10"/>
+      <c r="ES2" s="63"/>
+      <c r="ET2" s="10"/>
+      <c r="EU2" s="63"/>
+      <c r="EV2" s="10"/>
+      <c r="EW2" s="63"/>
+      <c r="EX2" s="10"/>
+      <c r="EY2" s="63"/>
+      <c r="EZ2" s="10"/>
+      <c r="FA2" s="63"/>
+      <c r="FB2" s="10"/>
+      <c r="FC2" s="63"/>
+      <c r="FD2" s="10"/>
+      <c r="FE2" s="63"/>
+      <c r="FF2" s="10"/>
+      <c r="FG2" s="63"/>
+      <c r="FH2" s="10"/>
+      <c r="FI2" s="63"/>
+      <c r="FJ2" s="10"/>
+      <c r="FK2" s="63"/>
+      <c r="FL2" s="10"/>
+      <c r="FM2" s="63"/>
+      <c r="FN2" s="10"/>
+      <c r="FO2" s="63"/>
+      <c r="FP2" s="10"/>
+      <c r="FQ2" s="63"/>
+      <c r="FR2" s="10"/>
+      <c r="FS2" s="63"/>
+      <c r="FT2" s="10"/>
+      <c r="FU2" s="63"/>
+      <c r="FV2" s="10"/>
+      <c r="FW2" s="63"/>
+      <c r="FX2" s="10"/>
+      <c r="FY2" s="63"/>
+      <c r="FZ2" s="10"/>
+      <c r="GA2" s="63"/>
+      <c r="GB2" s="10"/>
+      <c r="GC2" s="63"/>
+      <c r="GD2" s="10"/>
+      <c r="GE2" s="63"/>
+      <c r="GF2" s="10"/>
+      <c r="GG2" s="63"/>
+      <c r="GH2" s="10"/>
+      <c r="GI2" s="63"/>
+      <c r="GJ2" s="10"/>
+      <c r="GK2" s="63"/>
+      <c r="GL2" s="10"/>
+      <c r="GM2" s="63"/>
+      <c r="GN2" s="10"/>
+      <c r="GO2" s="63"/>
+      <c r="GP2" s="10"/>
+      <c r="GQ2" s="63"/>
+      <c r="GR2" s="10"/>
+      <c r="GS2" s="63"/>
+      <c r="GT2" s="10"/>
+      <c r="GU2" s="63"/>
+      <c r="GV2" s="10"/>
+      <c r="GW2" s="63"/>
+      <c r="GX2" s="10"/>
+      <c r="GY2" s="63"/>
+      <c r="GZ2" s="10"/>
+      <c r="HA2" s="63"/>
+      <c r="HB2" s="10"/>
+      <c r="HC2" s="63"/>
+      <c r="HD2" s="10"/>
+      <c r="HE2" s="63"/>
+      <c r="HF2" s="10"/>
+      <c r="HG2" s="63"/>
+      <c r="HH2" s="10"/>
+      <c r="HI2" s="63"/>
+      <c r="HJ2" s="10"/>
+      <c r="HK2" s="63"/>
+      <c r="HL2" s="10"/>
+      <c r="HM2" s="63"/>
+      <c r="HN2" s="10"/>
+      <c r="HO2" s="63"/>
+      <c r="HP2" s="10"/>
+      <c r="HQ2" s="63"/>
+      <c r="HR2" s="10"/>
+      <c r="HS2" s="63"/>
+      <c r="HT2" s="10"/>
+      <c r="HU2" s="63"/>
+      <c r="HV2" s="10"/>
+      <c r="HW2" s="63"/>
+      <c r="HX2" s="10"/>
+      <c r="HY2" s="63"/>
+      <c r="HZ2" s="10"/>
+      <c r="IA2" s="63"/>
+      <c r="IB2" s="10"/>
+      <c r="IC2" s="63"/>
+      <c r="ID2" s="10"/>
+      <c r="IE2" s="63"/>
+      <c r="IF2" s="10"/>
+      <c r="IG2" s="63"/>
+      <c r="IH2" s="10"/>
+      <c r="II2" s="63"/>
+      <c r="IJ2" s="10"/>
+      <c r="IK2" s="63"/>
+      <c r="IL2" s="10"/>
+      <c r="IM2" s="63"/>
+      <c r="IN2" s="10"/>
+      <c r="IO2" s="63"/>
+      <c r="IP2" s="10"/>
+      <c r="IQ2" s="63"/>
+      <c r="IR2" s="10"/>
+      <c r="IS2" s="63"/>
+      <c r="IT2" s="10"/>
+      <c r="IU2" s="63"/>
+      <c r="IV2" s="10"/>
+      <c r="IW2" s="63"/>
+      <c r="IX2" s="10"/>
+      <c r="IY2" s="63"/>
+      <c r="IZ2" s="10"/>
+      <c r="JA2" s="63"/>
+      <c r="JB2" s="10"/>
+      <c r="JC2" s="63"/>
+      <c r="JD2" s="10"/>
+      <c r="JE2" s="63"/>
+      <c r="JF2" s="10"/>
+      <c r="JG2" s="63"/>
+      <c r="JH2" s="10"/>
+      <c r="JI2" s="63"/>
+      <c r="JJ2" s="10"/>
+      <c r="JK2" s="63"/>
+      <c r="JL2" s="10"/>
+      <c r="JM2" s="63"/>
+      <c r="JN2" s="10"/>
+      <c r="JO2" s="63"/>
+      <c r="JP2" s="10"/>
+      <c r="JQ2" s="63"/>
+      <c r="JR2" s="10"/>
+      <c r="JS2" s="63"/>
+      <c r="JT2" s="10"/>
+      <c r="JU2" s="63"/>
+      <c r="JV2" s="10"/>
+      <c r="JW2" s="63"/>
+      <c r="JX2" s="10"/>
+      <c r="JY2" s="63"/>
+      <c r="JZ2" s="10"/>
+      <c r="KA2" s="63"/>
+      <c r="KB2" s="10"/>
+      <c r="KC2" s="63"/>
+      <c r="KD2" s="10"/>
+      <c r="KE2" s="63"/>
+      <c r="KF2" s="10"/>
+      <c r="KG2" s="63"/>
+      <c r="KH2" s="10"/>
+      <c r="KI2" s="63"/>
+      <c r="KJ2" s="10"/>
+      <c r="KK2" s="63"/>
+      <c r="KL2" s="10"/>
+      <c r="KM2" s="63"/>
+      <c r="KN2" s="10"/>
+      <c r="KO2" s="63"/>
+      <c r="KP2" s="10"/>
+      <c r="KQ2" s="63"/>
+      <c r="KR2" s="10"/>
+      <c r="KS2" s="63"/>
+      <c r="KT2" s="10"/>
+      <c r="KU2" s="63"/>
+      <c r="KV2" s="10"/>
+      <c r="KW2" s="63"/>
+      <c r="KX2" s="10"/>
+      <c r="KY2" s="63"/>
+      <c r="KZ2" s="10"/>
+      <c r="LA2" s="63"/>
+      <c r="LB2" s="10"/>
+      <c r="LC2" s="63"/>
+      <c r="LD2" s="10"/>
+      <c r="LE2" s="63"/>
+      <c r="LF2" s="10"/>
+      <c r="LG2" s="63"/>
+      <c r="LH2" s="10"/>
+      <c r="LI2" s="63"/>
+      <c r="LJ2" s="10"/>
+      <c r="LK2" s="63"/>
+      <c r="LL2" s="10"/>
+      <c r="LM2" s="63"/>
+      <c r="LN2" s="10"/>
+      <c r="LO2" s="63"/>
+      <c r="LP2" s="10"/>
+      <c r="LQ2" s="63"/>
+      <c r="LR2" s="10"/>
+      <c r="LS2" s="63"/>
+      <c r="LT2" s="10"/>
+      <c r="LU2" s="63"/>
+      <c r="LV2" s="10"/>
+      <c r="LW2" s="63"/>
+      <c r="LX2" s="10"/>
+      <c r="LY2" s="63"/>
+      <c r="LZ2" s="10"/>
+      <c r="MA2" s="63"/>
+      <c r="MB2" s="10"/>
+      <c r="MC2" s="63"/>
+      <c r="MD2" s="10"/>
+      <c r="ME2" s="63"/>
+      <c r="MF2" s="10"/>
+      <c r="MG2" s="63"/>
+      <c r="MH2" s="10"/>
+      <c r="MI2" s="63"/>
+      <c r="MJ2" s="10"/>
+      <c r="MK2" s="63"/>
+      <c r="ML2" s="10"/>
+      <c r="MM2" s="63"/>
+      <c r="MN2" s="10"/>
+      <c r="MO2" s="63"/>
+      <c r="MP2" s="10"/>
+      <c r="MQ2" s="63"/>
+      <c r="MR2" s="10"/>
+      <c r="MS2" s="63"/>
+      <c r="MT2" s="10"/>
+      <c r="MU2" s="63"/>
+      <c r="MV2" s="10"/>
+      <c r="MW2" s="63"/>
+      <c r="MX2" s="10"/>
+      <c r="MY2" s="63"/>
+      <c r="MZ2" s="10"/>
+      <c r="NA2" s="63"/>
+      <c r="NB2" s="10"/>
+      <c r="NC2" s="63"/>
+      <c r="ND2" s="10"/>
+      <c r="NE2" s="63"/>
+    </row>
+    <row r="3" spans="1:369">
       <c r="A3" s="60" t="s">
         <v>66</v>
       </c>
@@ -2127,23 +3236,775 @@
       </c>
       <c r="C3" s="64"/>
       <c r="D3" s="9">
+        <v>14</v>
+      </c>
+      <c r="E3" s="64"/>
+      <c r="F3" s="9">
+        <v>15</v>
+      </c>
+      <c r="G3" s="64"/>
+      <c r="H3" s="9">
+        <v>16</v>
+      </c>
+      <c r="I3" s="64"/>
+      <c r="J3" s="9">
+        <v>15</v>
+      </c>
+      <c r="K3" s="64"/>
+      <c r="L3" s="9">
+        <v>14</v>
+      </c>
+      <c r="M3" s="64"/>
+      <c r="N3" s="9">
         <v>13</v>
       </c>
-      <c r="E3" s="64"/>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="O3" s="64"/>
+      <c r="P3" s="9">
+        <v>13</v>
+      </c>
+      <c r="Q3" s="64"/>
+      <c r="R3" s="9"/>
+      <c r="S3" s="64"/>
+      <c r="T3" s="9"/>
+      <c r="U3" s="64"/>
+      <c r="V3" s="9"/>
+      <c r="W3" s="64"/>
+      <c r="X3" s="9"/>
+      <c r="Y3" s="64"/>
+      <c r="Z3" s="9"/>
+      <c r="AA3" s="64"/>
+      <c r="AB3" s="9"/>
+      <c r="AC3" s="64"/>
+      <c r="AD3" s="9"/>
+      <c r="AE3" s="64"/>
+      <c r="AF3" s="9"/>
+      <c r="AG3" s="64"/>
+      <c r="AH3" s="9"/>
+      <c r="AI3" s="64"/>
+      <c r="AJ3" s="9"/>
+      <c r="AK3" s="64"/>
+      <c r="AL3" s="9"/>
+      <c r="AM3" s="64"/>
+      <c r="AN3" s="9"/>
+      <c r="AO3" s="64"/>
+      <c r="AP3" s="9"/>
+      <c r="AQ3" s="64"/>
+      <c r="AR3" s="9"/>
+      <c r="AS3" s="64"/>
+      <c r="AT3" s="9"/>
+      <c r="AU3" s="64"/>
+      <c r="AV3" s="9"/>
+      <c r="AW3" s="64"/>
+      <c r="AX3" s="9"/>
+      <c r="AY3" s="64"/>
+      <c r="AZ3" s="9"/>
+      <c r="BA3" s="64"/>
+      <c r="BB3" s="9"/>
+      <c r="BC3" s="64"/>
+      <c r="BD3" s="9"/>
+      <c r="BE3" s="64"/>
+      <c r="BF3" s="9"/>
+      <c r="BG3" s="64"/>
+      <c r="BH3" s="9"/>
+      <c r="BI3" s="64"/>
+      <c r="BJ3" s="9"/>
+      <c r="BK3" s="64"/>
+      <c r="BL3" s="9"/>
+      <c r="BM3" s="64"/>
+      <c r="BN3" s="9"/>
+      <c r="BO3" s="64"/>
+      <c r="BP3" s="9"/>
+      <c r="BQ3" s="64"/>
+      <c r="BR3" s="9"/>
+      <c r="BS3" s="64"/>
+      <c r="BT3" s="9"/>
+      <c r="BU3" s="64"/>
+      <c r="BV3" s="9"/>
+      <c r="BW3" s="64"/>
+      <c r="BX3" s="9"/>
+      <c r="BY3" s="64"/>
+      <c r="BZ3" s="9"/>
+      <c r="CA3" s="64"/>
+      <c r="CB3" s="9"/>
+      <c r="CC3" s="64"/>
+      <c r="CD3" s="9"/>
+      <c r="CE3" s="64"/>
+      <c r="CF3" s="9"/>
+      <c r="CG3" s="64"/>
+      <c r="CH3" s="9"/>
+      <c r="CI3" s="64"/>
+      <c r="CJ3" s="9"/>
+      <c r="CK3" s="64"/>
+      <c r="CL3" s="9"/>
+      <c r="CM3" s="64"/>
+      <c r="CN3" s="9"/>
+      <c r="CO3" s="64"/>
+      <c r="CP3" s="9"/>
+      <c r="CQ3" s="64"/>
+      <c r="CR3" s="9"/>
+      <c r="CS3" s="64"/>
+      <c r="CT3" s="9"/>
+      <c r="CU3" s="64"/>
+      <c r="CV3" s="9"/>
+      <c r="CW3" s="64"/>
+      <c r="CX3" s="9"/>
+      <c r="CY3" s="64"/>
+      <c r="CZ3" s="9"/>
+      <c r="DA3" s="64"/>
+      <c r="DB3" s="9"/>
+      <c r="DC3" s="64"/>
+      <c r="DD3" s="9"/>
+      <c r="DE3" s="64"/>
+      <c r="DF3" s="9"/>
+      <c r="DG3" s="64"/>
+      <c r="DH3" s="9"/>
+      <c r="DI3" s="64"/>
+      <c r="DJ3" s="9"/>
+      <c r="DK3" s="64"/>
+      <c r="DL3" s="9"/>
+      <c r="DM3" s="64"/>
+      <c r="DN3" s="9"/>
+      <c r="DO3" s="64"/>
+      <c r="DP3" s="9"/>
+      <c r="DQ3" s="64"/>
+      <c r="DR3" s="9"/>
+      <c r="DS3" s="64"/>
+      <c r="DT3" s="9"/>
+      <c r="DU3" s="64"/>
+      <c r="DV3" s="9"/>
+      <c r="DW3" s="64"/>
+      <c r="DX3" s="9"/>
+      <c r="DY3" s="64"/>
+      <c r="DZ3" s="9"/>
+      <c r="EA3" s="64"/>
+      <c r="EB3" s="9"/>
+      <c r="EC3" s="64"/>
+      <c r="ED3" s="9"/>
+      <c r="EE3" s="64"/>
+      <c r="EF3" s="9"/>
+      <c r="EG3" s="64"/>
+      <c r="EH3" s="9"/>
+      <c r="EI3" s="64"/>
+      <c r="EJ3" s="9"/>
+      <c r="EK3" s="64"/>
+      <c r="EL3" s="9"/>
+      <c r="EM3" s="64"/>
+      <c r="EN3" s="9"/>
+      <c r="EO3" s="64"/>
+      <c r="EP3" s="9"/>
+      <c r="EQ3" s="64"/>
+      <c r="ER3" s="9"/>
+      <c r="ES3" s="64"/>
+      <c r="ET3" s="9"/>
+      <c r="EU3" s="64"/>
+      <c r="EV3" s="9"/>
+      <c r="EW3" s="64"/>
+      <c r="EX3" s="9"/>
+      <c r="EY3" s="64"/>
+      <c r="EZ3" s="9"/>
+      <c r="FA3" s="64"/>
+      <c r="FB3" s="9"/>
+      <c r="FC3" s="64"/>
+      <c r="FD3" s="9"/>
+      <c r="FE3" s="64"/>
+      <c r="FF3" s="9"/>
+      <c r="FG3" s="64"/>
+      <c r="FH3" s="9"/>
+      <c r="FI3" s="64"/>
+      <c r="FJ3" s="9"/>
+      <c r="FK3" s="64"/>
+      <c r="FL3" s="9"/>
+      <c r="FM3" s="64"/>
+      <c r="FN3" s="9"/>
+      <c r="FO3" s="64"/>
+      <c r="FP3" s="9"/>
+      <c r="FQ3" s="64"/>
+      <c r="FR3" s="9"/>
+      <c r="FS3" s="64"/>
+      <c r="FT3" s="9"/>
+      <c r="FU3" s="64"/>
+      <c r="FV3" s="9"/>
+      <c r="FW3" s="64"/>
+      <c r="FX3" s="9"/>
+      <c r="FY3" s="64"/>
+      <c r="FZ3" s="9"/>
+      <c r="GA3" s="64"/>
+      <c r="GB3" s="9"/>
+      <c r="GC3" s="64"/>
+      <c r="GD3" s="9"/>
+      <c r="GE3" s="64"/>
+      <c r="GF3" s="9"/>
+      <c r="GG3" s="64"/>
+      <c r="GH3" s="9"/>
+      <c r="GI3" s="64"/>
+      <c r="GJ3" s="9"/>
+      <c r="GK3" s="64"/>
+      <c r="GL3" s="9"/>
+      <c r="GM3" s="64"/>
+      <c r="GN3" s="9"/>
+      <c r="GO3" s="64"/>
+      <c r="GP3" s="9"/>
+      <c r="GQ3" s="64"/>
+      <c r="GR3" s="9"/>
+      <c r="GS3" s="64"/>
+      <c r="GT3" s="9"/>
+      <c r="GU3" s="64"/>
+      <c r="GV3" s="9"/>
+      <c r="GW3" s="64"/>
+      <c r="GX3" s="9"/>
+      <c r="GY3" s="64"/>
+      <c r="GZ3" s="9"/>
+      <c r="HA3" s="64"/>
+      <c r="HB3" s="9"/>
+      <c r="HC3" s="64"/>
+      <c r="HD3" s="9"/>
+      <c r="HE3" s="64"/>
+      <c r="HF3" s="9"/>
+      <c r="HG3" s="64"/>
+      <c r="HH3" s="9"/>
+      <c r="HI3" s="64"/>
+      <c r="HJ3" s="9"/>
+      <c r="HK3" s="64"/>
+      <c r="HL3" s="9"/>
+      <c r="HM3" s="64"/>
+      <c r="HN3" s="9"/>
+      <c r="HO3" s="64"/>
+      <c r="HP3" s="9"/>
+      <c r="HQ3" s="64"/>
+      <c r="HR3" s="9"/>
+      <c r="HS3" s="64"/>
+      <c r="HT3" s="9"/>
+      <c r="HU3" s="64"/>
+      <c r="HV3" s="9"/>
+      <c r="HW3" s="64"/>
+      <c r="HX3" s="9"/>
+      <c r="HY3" s="64"/>
+      <c r="HZ3" s="9"/>
+      <c r="IA3" s="64"/>
+      <c r="IB3" s="9"/>
+      <c r="IC3" s="64"/>
+      <c r="ID3" s="9"/>
+      <c r="IE3" s="64"/>
+      <c r="IF3" s="9"/>
+      <c r="IG3" s="64"/>
+      <c r="IH3" s="9"/>
+      <c r="II3" s="64"/>
+      <c r="IJ3" s="9"/>
+      <c r="IK3" s="64"/>
+      <c r="IL3" s="9"/>
+      <c r="IM3" s="64"/>
+      <c r="IN3" s="9"/>
+      <c r="IO3" s="64"/>
+      <c r="IP3" s="9"/>
+      <c r="IQ3" s="64"/>
+      <c r="IR3" s="9"/>
+      <c r="IS3" s="64"/>
+      <c r="IT3" s="9"/>
+      <c r="IU3" s="64"/>
+      <c r="IV3" s="9"/>
+      <c r="IW3" s="64"/>
+      <c r="IX3" s="9"/>
+      <c r="IY3" s="64"/>
+      <c r="IZ3" s="9"/>
+      <c r="JA3" s="64"/>
+      <c r="JB3" s="9"/>
+      <c r="JC3" s="64"/>
+      <c r="JD3" s="9"/>
+      <c r="JE3" s="64"/>
+      <c r="JF3" s="9"/>
+      <c r="JG3" s="64"/>
+      <c r="JH3" s="9"/>
+      <c r="JI3" s="64"/>
+      <c r="JJ3" s="9"/>
+      <c r="JK3" s="64"/>
+      <c r="JL3" s="9"/>
+      <c r="JM3" s="64"/>
+      <c r="JN3" s="9"/>
+      <c r="JO3" s="64"/>
+      <c r="JP3" s="9"/>
+      <c r="JQ3" s="64"/>
+      <c r="JR3" s="9"/>
+      <c r="JS3" s="64"/>
+      <c r="JT3" s="9"/>
+      <c r="JU3" s="64"/>
+      <c r="JV3" s="9"/>
+      <c r="JW3" s="64"/>
+      <c r="JX3" s="9"/>
+      <c r="JY3" s="64"/>
+      <c r="JZ3" s="9"/>
+      <c r="KA3" s="64"/>
+      <c r="KB3" s="9"/>
+      <c r="KC3" s="64"/>
+      <c r="KD3" s="9"/>
+      <c r="KE3" s="64"/>
+      <c r="KF3" s="9"/>
+      <c r="KG3" s="64"/>
+      <c r="KH3" s="9"/>
+      <c r="KI3" s="64"/>
+      <c r="KJ3" s="9"/>
+      <c r="KK3" s="64"/>
+      <c r="KL3" s="9"/>
+      <c r="KM3" s="64"/>
+      <c r="KN3" s="9"/>
+      <c r="KO3" s="64"/>
+      <c r="KP3" s="9"/>
+      <c r="KQ3" s="64"/>
+      <c r="KR3" s="9"/>
+      <c r="KS3" s="64"/>
+      <c r="KT3" s="9"/>
+      <c r="KU3" s="64"/>
+      <c r="KV3" s="9"/>
+      <c r="KW3" s="64"/>
+      <c r="KX3" s="9"/>
+      <c r="KY3" s="64"/>
+      <c r="KZ3" s="9"/>
+      <c r="LA3" s="64"/>
+      <c r="LB3" s="9"/>
+      <c r="LC3" s="64"/>
+      <c r="LD3" s="9"/>
+      <c r="LE3" s="64"/>
+      <c r="LF3" s="9"/>
+      <c r="LG3" s="64"/>
+      <c r="LH3" s="9"/>
+      <c r="LI3" s="64"/>
+      <c r="LJ3" s="9"/>
+      <c r="LK3" s="64"/>
+      <c r="LL3" s="9"/>
+      <c r="LM3" s="64"/>
+      <c r="LN3" s="9"/>
+      <c r="LO3" s="64"/>
+      <c r="LP3" s="9"/>
+      <c r="LQ3" s="64"/>
+      <c r="LR3" s="9"/>
+      <c r="LS3" s="64"/>
+      <c r="LT3" s="9"/>
+      <c r="LU3" s="64"/>
+      <c r="LV3" s="9"/>
+      <c r="LW3" s="64"/>
+      <c r="LX3" s="9"/>
+      <c r="LY3" s="64"/>
+      <c r="LZ3" s="9"/>
+      <c r="MA3" s="64"/>
+      <c r="MB3" s="9"/>
+      <c r="MC3" s="64"/>
+      <c r="MD3" s="9"/>
+      <c r="ME3" s="64"/>
+      <c r="MF3" s="9"/>
+      <c r="MG3" s="64"/>
+      <c r="MH3" s="9"/>
+      <c r="MI3" s="64"/>
+      <c r="MJ3" s="9"/>
+      <c r="MK3" s="64"/>
+      <c r="ML3" s="9"/>
+      <c r="MM3" s="64"/>
+      <c r="MN3" s="9"/>
+      <c r="MO3" s="64"/>
+      <c r="MP3" s="9"/>
+      <c r="MQ3" s="64"/>
+      <c r="MR3" s="9"/>
+      <c r="MS3" s="64"/>
+      <c r="MT3" s="9"/>
+      <c r="MU3" s="64"/>
+      <c r="MV3" s="9"/>
+      <c r="MW3" s="64"/>
+      <c r="MX3" s="9"/>
+      <c r="MY3" s="64"/>
+      <c r="MZ3" s="9"/>
+      <c r="NA3" s="64"/>
+      <c r="NB3" s="9"/>
+      <c r="NC3" s="64"/>
+      <c r="ND3" s="9"/>
+      <c r="NE3" s="64"/>
+    </row>
+    <row r="4" spans="1:369">
       <c r="A4" s="35"/>
       <c r="B4" s="35"/>
       <c r="C4" s="35"/>
       <c r="D4" s="35"/>
       <c r="E4" s="35"/>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="35"/>
+      <c r="K4" s="35"/>
+      <c r="L4" s="35"/>
+      <c r="M4" s="35"/>
+      <c r="N4" s="35"/>
+      <c r="O4" s="35"/>
+      <c r="P4" s="35"/>
+      <c r="Q4" s="35"/>
+      <c r="R4" s="35"/>
+      <c r="S4" s="35"/>
+      <c r="T4" s="35"/>
+      <c r="U4" s="35"/>
+      <c r="V4" s="35"/>
+      <c r="W4" s="35"/>
+      <c r="X4" s="35"/>
+      <c r="Y4" s="35"/>
+      <c r="Z4" s="35"/>
+      <c r="AA4" s="35"/>
+      <c r="AB4" s="35"/>
+      <c r="AC4" s="35"/>
+      <c r="AD4" s="35"/>
+      <c r="AE4" s="35"/>
+      <c r="AF4" s="35"/>
+      <c r="AG4" s="35"/>
+      <c r="AH4" s="35"/>
+      <c r="AI4" s="35"/>
+      <c r="AJ4" s="35"/>
+      <c r="AK4" s="35"/>
+      <c r="AL4" s="35"/>
+      <c r="AM4" s="35"/>
+      <c r="AN4" s="35"/>
+      <c r="AO4" s="35"/>
+      <c r="AP4" s="35"/>
+      <c r="AQ4" s="35"/>
+      <c r="AR4" s="35"/>
+      <c r="AS4" s="35"/>
+      <c r="AT4" s="35"/>
+      <c r="AU4" s="35"/>
+      <c r="AV4" s="35"/>
+      <c r="AW4" s="35"/>
+      <c r="AX4" s="35"/>
+      <c r="AY4" s="35"/>
+      <c r="AZ4" s="35"/>
+      <c r="BA4" s="35"/>
+      <c r="BB4" s="35"/>
+      <c r="BC4" s="35"/>
+      <c r="BD4" s="35"/>
+      <c r="BE4" s="35"/>
+      <c r="BF4" s="35"/>
+      <c r="BG4" s="35"/>
+      <c r="BH4" s="35"/>
+      <c r="BI4" s="35"/>
+      <c r="BJ4" s="35"/>
+      <c r="BK4" s="35"/>
+      <c r="BL4" s="35"/>
+      <c r="BM4" s="35"/>
+      <c r="BN4" s="35"/>
+      <c r="BO4" s="35"/>
+      <c r="BP4" s="35"/>
+      <c r="BQ4" s="35"/>
+      <c r="BR4" s="35"/>
+      <c r="BS4" s="35"/>
+      <c r="BT4" s="35"/>
+      <c r="BU4" s="35"/>
+      <c r="BV4" s="35"/>
+      <c r="BW4" s="35"/>
+      <c r="BX4" s="35"/>
+      <c r="BY4" s="35"/>
+      <c r="BZ4" s="35"/>
+      <c r="CA4" s="35"/>
+      <c r="CB4" s="35"/>
+      <c r="CC4" s="35"/>
+      <c r="CD4" s="35"/>
+      <c r="CE4" s="35"/>
+      <c r="CF4" s="35"/>
+      <c r="CG4" s="35"/>
+      <c r="CH4" s="35"/>
+      <c r="CI4" s="35"/>
+      <c r="CJ4" s="35"/>
+      <c r="CK4" s="35"/>
+      <c r="CL4" s="35"/>
+      <c r="CM4" s="35"/>
+      <c r="CN4" s="35"/>
+      <c r="CO4" s="35"/>
+      <c r="CP4" s="35"/>
+      <c r="CQ4" s="35"/>
+      <c r="CR4" s="35"/>
+      <c r="CS4" s="35"/>
+      <c r="CT4" s="35"/>
+      <c r="CU4" s="35"/>
+      <c r="CV4" s="35"/>
+      <c r="CW4" s="35"/>
+      <c r="CX4" s="35"/>
+      <c r="CY4" s="35"/>
+      <c r="CZ4" s="35"/>
+      <c r="DA4" s="35"/>
+      <c r="DB4" s="35"/>
+      <c r="DC4" s="35"/>
+      <c r="DD4" s="35"/>
+      <c r="DE4" s="35"/>
+      <c r="DF4" s="35"/>
+      <c r="DG4" s="35"/>
+      <c r="DH4" s="35"/>
+      <c r="DI4" s="35"/>
+      <c r="DJ4" s="35"/>
+      <c r="DK4" s="35"/>
+      <c r="DL4" s="35"/>
+      <c r="DM4" s="35"/>
+      <c r="DN4" s="35"/>
+      <c r="DO4" s="35"/>
+      <c r="DP4" s="35"/>
+      <c r="DQ4" s="35"/>
+      <c r="DR4" s="35"/>
+      <c r="DS4" s="35"/>
+      <c r="DT4" s="35"/>
+      <c r="DU4" s="35"/>
+      <c r="DV4" s="35"/>
+      <c r="DW4" s="35"/>
+      <c r="DX4" s="35"/>
+      <c r="DY4" s="35"/>
+      <c r="DZ4" s="35"/>
+      <c r="EA4" s="35"/>
+      <c r="EB4" s="35"/>
+      <c r="EC4" s="35"/>
+      <c r="ED4" s="35"/>
+      <c r="EE4" s="35"/>
+      <c r="EF4" s="35"/>
+      <c r="EG4" s="35"/>
+      <c r="EH4" s="35"/>
+      <c r="EI4" s="35"/>
+      <c r="EJ4" s="35"/>
+      <c r="EK4" s="35"/>
+      <c r="EL4" s="35"/>
+      <c r="EM4" s="35"/>
+      <c r="EN4" s="35"/>
+      <c r="EO4" s="35"/>
+      <c r="EP4" s="35"/>
+      <c r="EQ4" s="35"/>
+      <c r="ER4" s="35"/>
+      <c r="ES4" s="35"/>
+      <c r="ET4" s="35"/>
+      <c r="EU4" s="35"/>
+      <c r="EV4" s="35"/>
+      <c r="EW4" s="35"/>
+      <c r="EX4" s="35"/>
+      <c r="EY4" s="35"/>
+      <c r="EZ4" s="35"/>
+      <c r="FA4" s="35"/>
+      <c r="FB4" s="35"/>
+      <c r="FC4" s="35"/>
+      <c r="FD4" s="35"/>
+      <c r="FE4" s="35"/>
+      <c r="FF4" s="35"/>
+      <c r="FG4" s="35"/>
+      <c r="FH4" s="35"/>
+      <c r="FI4" s="35"/>
+      <c r="FJ4" s="35"/>
+      <c r="FK4" s="35"/>
+      <c r="FL4" s="35"/>
+      <c r="FM4" s="35"/>
+      <c r="FN4" s="35"/>
+      <c r="FO4" s="35"/>
+      <c r="FP4" s="35"/>
+      <c r="FQ4" s="35"/>
+      <c r="FR4" s="35"/>
+      <c r="FS4" s="35"/>
+      <c r="FT4" s="35"/>
+      <c r="FU4" s="35"/>
+      <c r="FV4" s="35"/>
+      <c r="FW4" s="35"/>
+      <c r="FX4" s="35"/>
+      <c r="FY4" s="35"/>
+      <c r="FZ4" s="35"/>
+      <c r="GA4" s="35"/>
+      <c r="GB4" s="35"/>
+      <c r="GC4" s="35"/>
+      <c r="GD4" s="35"/>
+      <c r="GE4" s="35"/>
+      <c r="GF4" s="35"/>
+      <c r="GG4" s="35"/>
+      <c r="GH4" s="35"/>
+      <c r="GI4" s="35"/>
+      <c r="GJ4" s="35"/>
+      <c r="GK4" s="35"/>
+    </row>
+    <row r="5" spans="1:369">
       <c r="A5" s="35"/>
       <c r="B5" s="35"/>
       <c r="C5" s="35"/>
       <c r="D5" s="35"/>
       <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="35"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="35"/>
+      <c r="K5" s="35"/>
+      <c r="L5" s="35"/>
+      <c r="M5" s="35"/>
+      <c r="N5" s="35"/>
+      <c r="O5" s="35"/>
+      <c r="P5" s="35"/>
+      <c r="Q5" s="35"/>
+      <c r="R5" s="35"/>
+      <c r="S5" s="35"/>
+      <c r="T5" s="35"/>
+      <c r="U5" s="35"/>
+      <c r="V5" s="35"/>
+      <c r="W5" s="35"/>
+      <c r="X5" s="35"/>
+      <c r="Y5" s="35"/>
+      <c r="Z5" s="35"/>
+      <c r="AA5" s="35"/>
+      <c r="AB5" s="35"/>
+      <c r="AC5" s="35"/>
+      <c r="AD5" s="35"/>
+      <c r="AE5" s="35"/>
+      <c r="AF5" s="35"/>
+      <c r="AG5" s="35"/>
+      <c r="AH5" s="35"/>
+      <c r="AI5" s="35"/>
+      <c r="AJ5" s="35"/>
+      <c r="AK5" s="35"/>
+      <c r="AL5" s="35"/>
+      <c r="AM5" s="35"/>
+      <c r="AN5" s="35"/>
+      <c r="AO5" s="35"/>
+      <c r="AP5" s="35"/>
+      <c r="AQ5" s="35"/>
+      <c r="AR5" s="35"/>
+      <c r="AS5" s="35"/>
+      <c r="AT5" s="35"/>
+      <c r="AU5" s="35"/>
+      <c r="AV5" s="35"/>
+      <c r="AW5" s="35"/>
+      <c r="AX5" s="35"/>
+      <c r="AY5" s="35"/>
+      <c r="AZ5" s="35"/>
+      <c r="BA5" s="35"/>
+      <c r="BB5" s="35"/>
+      <c r="BC5" s="35"/>
+      <c r="BD5" s="35"/>
+      <c r="BE5" s="35"/>
+      <c r="BF5" s="35"/>
+      <c r="BG5" s="35"/>
+      <c r="BH5" s="35"/>
+      <c r="BI5" s="35"/>
+      <c r="BJ5" s="35"/>
+      <c r="BK5" s="35"/>
+      <c r="BL5" s="35"/>
+      <c r="BM5" s="35"/>
+      <c r="BN5" s="35"/>
+      <c r="BO5" s="35"/>
+      <c r="BP5" s="35"/>
+      <c r="BQ5" s="35"/>
+      <c r="BR5" s="35"/>
+      <c r="BS5" s="35"/>
+      <c r="BT5" s="35"/>
+      <c r="BU5" s="35"/>
+      <c r="BV5" s="35"/>
+      <c r="BW5" s="35"/>
+      <c r="BX5" s="35"/>
+      <c r="BY5" s="35"/>
+      <c r="BZ5" s="35"/>
+      <c r="CA5" s="35"/>
+      <c r="CB5" s="35"/>
+      <c r="CC5" s="35"/>
+      <c r="CD5" s="35"/>
+      <c r="CE5" s="35"/>
+      <c r="CF5" s="35"/>
+      <c r="CG5" s="35"/>
+      <c r="CH5" s="35"/>
+      <c r="CI5" s="35"/>
+      <c r="CJ5" s="35"/>
+      <c r="CK5" s="35"/>
+      <c r="CL5" s="35"/>
+      <c r="CM5" s="35"/>
+      <c r="CN5" s="35"/>
+      <c r="CO5" s="35"/>
+      <c r="CP5" s="35"/>
+      <c r="CQ5" s="35"/>
+      <c r="CR5" s="35"/>
+      <c r="CS5" s="35"/>
+      <c r="CT5" s="35"/>
+      <c r="CU5" s="35"/>
+      <c r="CV5" s="35"/>
+      <c r="CW5" s="35"/>
+      <c r="CX5" s="35"/>
+      <c r="CY5" s="35"/>
+      <c r="CZ5" s="35"/>
+      <c r="DA5" s="35"/>
+      <c r="DB5" s="35"/>
+      <c r="DC5" s="35"/>
+      <c r="DD5" s="35"/>
+      <c r="DE5" s="35"/>
+      <c r="DF5" s="35"/>
+      <c r="DG5" s="35"/>
+      <c r="DH5" s="35"/>
+      <c r="DI5" s="35"/>
+      <c r="DJ5" s="35"/>
+      <c r="DK5" s="35"/>
+      <c r="DL5" s="35"/>
+      <c r="DM5" s="35"/>
+      <c r="DN5" s="35"/>
+      <c r="DO5" s="35"/>
+      <c r="DP5" s="35"/>
+      <c r="DQ5" s="35"/>
+      <c r="DR5" s="35"/>
+      <c r="DS5" s="35"/>
+      <c r="DT5" s="35"/>
+      <c r="DU5" s="35"/>
+      <c r="DV5" s="35"/>
+      <c r="DW5" s="35"/>
+      <c r="DX5" s="35"/>
+      <c r="DY5" s="35"/>
+      <c r="DZ5" s="35"/>
+      <c r="EA5" s="35"/>
+      <c r="EB5" s="35"/>
+      <c r="EC5" s="35"/>
+      <c r="ED5" s="35"/>
+      <c r="EE5" s="35"/>
+      <c r="EF5" s="35"/>
+      <c r="EG5" s="35"/>
+      <c r="EH5" s="35"/>
+      <c r="EI5" s="35"/>
+      <c r="EJ5" s="35"/>
+      <c r="EK5" s="35"/>
+      <c r="EL5" s="35"/>
+      <c r="EM5" s="35"/>
+      <c r="EN5" s="35"/>
+      <c r="EO5" s="35"/>
+      <c r="EP5" s="35"/>
+      <c r="EQ5" s="35"/>
+      <c r="ER5" s="35"/>
+      <c r="ES5" s="35"/>
+      <c r="ET5" s="35"/>
+      <c r="EU5" s="35"/>
+      <c r="EV5" s="35"/>
+      <c r="EW5" s="35"/>
+      <c r="EX5" s="35"/>
+      <c r="EY5" s="35"/>
+      <c r="EZ5" s="35"/>
+      <c r="FA5" s="35"/>
+      <c r="FB5" s="35"/>
+      <c r="FC5" s="35"/>
+      <c r="FD5" s="35"/>
+      <c r="FE5" s="35"/>
+      <c r="FF5" s="35"/>
+      <c r="FG5" s="35"/>
+      <c r="FH5" s="35"/>
+      <c r="FI5" s="35"/>
+      <c r="FJ5" s="35"/>
+      <c r="FK5" s="35"/>
+      <c r="FL5" s="35"/>
+      <c r="FM5" s="35"/>
+      <c r="FN5" s="35"/>
+      <c r="FO5" s="35"/>
+      <c r="FP5" s="35"/>
+      <c r="FQ5" s="35"/>
+      <c r="FR5" s="35"/>
+      <c r="FS5" s="35"/>
+      <c r="FT5" s="35"/>
+      <c r="FU5" s="35"/>
+      <c r="FV5" s="35"/>
+      <c r="FW5" s="35"/>
+      <c r="FX5" s="35"/>
+      <c r="FY5" s="35"/>
+      <c r="FZ5" s="35"/>
+      <c r="GA5" s="35"/>
+      <c r="GB5" s="35"/>
+      <c r="GC5" s="35"/>
+      <c r="GD5" s="35"/>
+      <c r="GE5" s="35"/>
+      <c r="GF5" s="35"/>
+      <c r="GG5" s="35"/>
+      <c r="GH5" s="35"/>
+      <c r="GI5" s="35"/>
+      <c r="GJ5" s="35"/>
+      <c r="GK5" s="35"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2161,7 +4022,7 @@
   <dimension ref="A1:S145"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3143,8 +5004,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IJ229"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3694,17 +5555,21 @@
       <c r="A3" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="30">
-        <v>3.4000000000000002E-2</v>
-      </c>
-      <c r="C3" s="19"/>
+      <c r="B3" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="C3" s="30" t="s">
+        <v>89</v>
+      </c>
       <c r="D3" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="57">
-        <v>5.7000000000000001E-8</v>
-      </c>
-      <c r="F3" s="25"/>
+      <c r="E3" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="F3" s="57" t="s">
+        <v>88</v>
+      </c>
       <c r="G3" s="30">
         <v>0.08</v>
       </c>
@@ -3969,10 +5834,12 @@
       <c r="H4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I4" s="19">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="J4" s="19"/>
+      <c r="I4" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="J4" s="19" t="s">
+        <v>86</v>
+      </c>
       <c r="K4" s="33"/>
       <c r="L4" s="33"/>
       <c r="M4" s="33"/>
@@ -4218,7 +6085,7 @@
         <v>24</v>
       </c>
       <c r="E5" s="19"/>
-      <c r="F5" s="25"/>
+      <c r="F5" s="30"/>
       <c r="G5" s="7"/>
       <c r="H5" s="6" t="s">
         <v>25</v>

</xml_diff>